<commit_message>
up checkout, Test suite and collection & report
</commit_message>
<xml_diff>
--- a/Resources/ddt saucedemo.xlsx
+++ b/Resources/ddt saucedemo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="630" windowWidth="19815" windowHeight="9405"/>
+    <workbookView xWindow="390" yWindow="630" windowWidth="19815" windowHeight="9405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -95,10 +95,10 @@
     <t>Test.allTheThings() T-Shirt (Red)</t>
   </si>
   <si>
-    <t>$7.99</t>
-  </si>
-  <si>
-    <t>$49.99</t>
+    <t>Sauce Labs Onesie</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
   </si>
 </sst>
 </file>
@@ -128,10 +128,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF132322"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -379,7 +377,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -515,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -528,72 +526,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>